<commit_message>
tomar capturas y uat
</commit_message>
<xml_diff>
--- a/CuentasUAT.xlsx
+++ b/CuentasUAT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="13155" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="13155" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="390">
   <si>
     <t>Descripción</t>
   </si>
@@ -1070,9 +1070,6 @@
     <t>ht@gmail.com</t>
   </si>
   <si>
-    <t>55555550</t>
-  </si>
-  <si>
     <t>Habilitacion</t>
   </si>
   <si>
@@ -1151,9 +1148,6 @@
     <t>ceronewton@gmail.com</t>
   </si>
   <si>
-    <t>Cero</t>
-  </si>
-  <si>
     <t>Newton</t>
   </si>
   <si>
@@ -1163,28 +1157,46 @@
     <t>22222001</t>
   </si>
   <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Alta Linea Existe OfCom Debito</t>
+  </si>
+  <si>
+    <t>BBVA BANCO FRANCES SA</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>4487790000000018</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
     <t>22222002</t>
   </si>
   <si>
-    <t>22222003</t>
-  </si>
-  <si>
-    <t>22222004</t>
-  </si>
-  <si>
-    <t>22222005</t>
-  </si>
-  <si>
-    <t>22222006</t>
-  </si>
-  <si>
-    <t>22222007</t>
-  </si>
-  <si>
-    <t>22222008</t>
-  </si>
-  <si>
-    <t>22222009</t>
+    <t>2944675396</t>
+  </si>
+  <si>
+    <t>Dos</t>
+  </si>
+  <si>
+    <t>Linea Equipo Existe SPU</t>
+  </si>
+  <si>
+    <t>Galaxy - s8</t>
+  </si>
+  <si>
+    <t>ciudad autonoma de buenos aires</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1429,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1470,12 +1482,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1881,7 +1890,7 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2031,14 +2040,14 @@
         <v>114</v>
       </c>
       <c r="H8" t="s">
+        <v>367</v>
+      </c>
+      <c r="I8" t="s">
         <v>368</v>
-      </c>
-      <c r="I8" t="s">
-        <v>369</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="31"/>
-      <c r="L8" s="42"/>
+      <c r="L8" s="39"/>
       <c r="M8" s="31"/>
       <c r="N8" s="31"/>
     </row>
@@ -2046,54 +2055,54 @@
       <c r="A9" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="B9" s="52" t="s">
-        <v>370</v>
+      <c r="B9" s="49" t="s">
+        <v>369</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D9" t="s">
         <v>114</v>
       </c>
       <c r="E9" t="s">
+        <v>367</v>
+      </c>
+      <c r="F9" t="s">
         <v>368</v>
-      </c>
-      <c r="F9" t="s">
-        <v>369</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="31"/>
-      <c r="L9" s="42"/>
+      <c r="L9" s="39"/>
       <c r="M9" s="31"/>
       <c r="N9" s="31"/>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="49" t="s">
+        <v>370</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>369</v>
+      </c>
+      <c r="D10" s="49" t="s">
         <v>371</v>
       </c>
-      <c r="C10" s="52" t="s">
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="B11" s="49" t="s">
         <v>370</v>
       </c>
-      <c r="D10" s="52" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
-        <v>305</v>
-      </c>
-      <c r="B11" s="52" t="s">
-        <v>371</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>370</v>
-      </c>
-      <c r="D11" s="52" t="s">
-        <v>372</v>
+      <c r="C11" s="49" t="s">
+        <v>375</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -2114,10 +2123,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2219,10 +2228,10 @@
         <v>114</v>
       </c>
       <c r="I2" t="s">
+        <v>367</v>
+      </c>
+      <c r="J2" t="s">
         <v>368</v>
-      </c>
-      <c r="J2" t="s">
-        <v>369</v>
       </c>
       <c r="K2" s="32" t="s">
         <v>320</v>
@@ -2236,7 +2245,7 @@
       <c r="N2" s="31" t="s">
         <v>307</v>
       </c>
-      <c r="O2" s="42" t="s">
+      <c r="O2" s="39" t="s">
         <v>308</v>
       </c>
       <c r="P2" s="31" t="s">
@@ -2272,10 +2281,10 @@
         <v>114</v>
       </c>
       <c r="I3" t="s">
+        <v>367</v>
+      </c>
+      <c r="J3" t="s">
         <v>368</v>
-      </c>
-      <c r="J3" t="s">
-        <v>369</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="32"/>
@@ -2290,7 +2299,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D4">
         <v>52486595</v>
@@ -2337,10 +2346,10 @@
         <v>114</v>
       </c>
       <c r="I5" t="s">
+        <v>367</v>
+      </c>
+      <c r="J5" t="s">
         <v>368</v>
-      </c>
-      <c r="J5" t="s">
-        <v>369</v>
       </c>
       <c r="K5" s="32" t="s">
         <v>290</v>
@@ -2356,13 +2365,13 @@
         <v>306</v>
       </c>
       <c r="B6" s="31" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" t="s">
         <v>351</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>352</v>
-      </c>
-      <c r="D6" t="s">
-        <v>353</v>
       </c>
       <c r="E6" t="s">
         <v>276</v>
@@ -2377,15 +2386,15 @@
         <v>114</v>
       </c>
       <c r="I6" t="s">
+        <v>367</v>
+      </c>
+      <c r="J6" t="s">
         <v>368</v>
-      </c>
-      <c r="J6" t="s">
-        <v>369</v>
       </c>
       <c r="K6" s="31" t="s">
         <v>307</v>
       </c>
-      <c r="L6" s="42" t="s">
+      <c r="L6" s="39" t="s">
         <v>308</v>
       </c>
       <c r="M6" s="31" t="s">
@@ -2397,16 +2406,16 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B7">
         <v>59886004</v>
       </c>
       <c r="C7" t="s">
+        <v>353</v>
+      </c>
+      <c r="D7" t="s">
         <v>354</v>
-      </c>
-      <c r="D7" t="s">
-        <v>355</v>
       </c>
       <c r="E7" t="s">
         <v>276</v>
@@ -2415,7 +2424,7 @@
         <v>288</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H7" t="s">
         <v>114</v>
@@ -2424,7 +2433,7 @@
         <v>279</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>320</v>
@@ -2435,7 +2444,7 @@
       <c r="M7">
         <v>1524</v>
       </c>
-      <c r="N7" s="41" t="s">
+      <c r="N7" s="38" t="s">
         <v>332</v>
       </c>
       <c r="O7" s="31" t="s">
@@ -2461,14 +2470,14 @@
       </c>
       <c r="V7" s="31"/>
       <c r="W7" s="31"/>
-      <c r="X7" s="44"/>
+      <c r="X7" s="41"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>341</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C8" t="s">
         <v>344</v>
@@ -2489,10 +2498,10 @@
         <v>114</v>
       </c>
       <c r="I8" t="s">
+        <v>367</v>
+      </c>
+      <c r="J8" t="s">
         <v>368</v>
-      </c>
-      <c r="J8" t="s">
-        <v>369</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>320</v>
@@ -2510,10 +2519,10 @@
       </c>
       <c r="B9" s="32"/>
       <c r="C9" t="s">
+        <v>357</v>
+      </c>
+      <c r="D9" t="s">
         <v>358</v>
-      </c>
-      <c r="D9" t="s">
-        <v>359</v>
       </c>
       <c r="E9" t="s">
         <v>276</v>
@@ -2528,10 +2537,10 @@
         <v>114</v>
       </c>
       <c r="I9" t="s">
+        <v>367</v>
+      </c>
+      <c r="J9" t="s">
         <v>368</v>
-      </c>
-      <c r="J9" t="s">
-        <v>369</v>
       </c>
       <c r="K9" s="31" t="s">
         <v>320</v>
@@ -2542,7 +2551,7 @@
       <c r="M9">
         <v>1524</v>
       </c>
-      <c r="N9" s="41" t="s">
+      <c r="N9" s="38" t="s">
         <v>332</v>
       </c>
       <c r="O9" s="31" t="s">
@@ -2572,7 +2581,7 @@
       <c r="W9" s="31" t="s">
         <v>329</v>
       </c>
-      <c r="X9" s="44" t="s">
+      <c r="X9" s="41" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2580,34 +2589,87 @@
       <c r="A10" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="B10" s="52" t="s">
-        <v>370</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>374</v>
+      <c r="B10" s="49" t="s">
+        <v>384</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>386</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>276</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H10" t="s">
         <v>114</v>
       </c>
       <c r="I10" t="s">
+        <v>367</v>
+      </c>
+      <c r="J10" t="s">
         <v>368</v>
       </c>
-      <c r="J10" t="s">
-        <v>369</v>
-      </c>
-      <c r="K10" s="47"/>
+      <c r="K10" s="44"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>384</v>
+      </c>
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>378</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>379</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>331</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>380</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>381</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>382</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>383</v>
+      </c>
+      <c r="K11" s="31"/>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>384</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>389</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4465,8 +4527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4522,21 +4584,21 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="B2" s="38">
-        <v>46534534</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>295</v>
-      </c>
-      <c r="D2" s="37" t="s">
+      <c r="B2" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>297</v>
       </c>
-      <c r="E2" s="39">
-        <v>1158423198</v>
+      <c r="E2" s="49" t="s">
+        <v>371</v>
       </c>
       <c r="F2">
         <v>1161138551</v>
@@ -4546,11 +4608,11 @@
       <c r="A3" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="B3" s="36">
-        <v>23444455</v>
-      </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
+      <c r="B3" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
       <c r="G3">
         <v>1161138552</v>
       </c>
@@ -4559,30 +4621,30 @@
       <c r="A4" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C4" s="49" t="s">
         <v>370</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="D4" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="E4" s="49" t="s">
         <v>371</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>297</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>300</v>
       </c>
-      <c r="B5" s="53" t="s">
-        <v>377</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>371</v>
-      </c>
-      <c r="D5" s="41" t="s">
+      <c r="B5" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5" s="38" t="s">
         <v>332</v>
       </c>
       <c r="E5" s="31" t="s">
@@ -4620,53 +4682,53 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="40" t="s">
         <v>313</v>
       </c>
-      <c r="B6" s="53" t="s">
-        <v>378</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>371</v>
-      </c>
-      <c r="D6" s="45" t="s">
-        <v>362</v>
-      </c>
-      <c r="E6" s="49" t="s">
+      <c r="B6" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>370</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="E6" s="46" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="40" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="53" t="s">
-        <v>379</v>
-      </c>
-      <c r="C7" s="52" t="s">
-        <v>371</v>
-      </c>
-      <c r="D7" s="45" t="s">
-        <v>362</v>
-      </c>
-      <c r="E7" s="49" t="s">
+      <c r="B7" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>370</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="E7" s="46" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="40" t="s">
         <v>315</v>
       </c>
-      <c r="B8" s="53" t="s">
-        <v>380</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>371</v>
-      </c>
-      <c r="D8" s="45" t="s">
+      <c r="B8" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>370</v>
+      </c>
+      <c r="D8" s="42" t="s">
         <v>311</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="43" t="s">
         <v>312</v>
       </c>
       <c r="F8" t="s">
@@ -4677,14 +4739,14 @@
       <c r="A9" s="31" t="s">
         <v>317</v>
       </c>
-      <c r="B9" s="53" t="s">
-        <v>381</v>
-      </c>
-      <c r="C9" s="52" t="s">
+      <c r="B9" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>376</v>
+      </c>
+      <c r="D9" s="49" t="s">
         <v>371</v>
-      </c>
-      <c r="D9" s="52" t="s">
-        <v>372</v>
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
@@ -4699,38 +4761,38 @@
       <c r="O9" s="14"/>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="40" t="s">
         <v>318</v>
       </c>
-      <c r="B10" s="53" t="s">
-        <v>382</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>371</v>
+      <c r="B10" s="50" t="s">
+        <v>375</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="40" t="s">
         <v>319</v>
       </c>
-      <c r="B11" s="53" t="s">
-        <v>383</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>371</v>
+      <c r="B11" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="40" t="s">
         <v>328</v>
       </c>
-      <c r="B12" s="53" t="s">
-        <v>384</v>
-      </c>
-      <c r="C12" s="52" t="s">
-        <v>371</v>
-      </c>
-      <c r="D12" s="41" t="s">
+      <c r="B12" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>370</v>
+      </c>
+      <c r="D12" s="38" t="s">
         <v>332</v>
       </c>
       <c r="E12" s="31" t="s">
@@ -4757,59 +4819,62 @@
       <c r="L12" s="31" t="s">
         <v>301</v>
       </c>
-      <c r="M12" s="37" t="s">
-        <v>361</v>
-      </c>
-      <c r="N12" s="50" t="s">
-        <v>367</v>
+      <c r="M12" s="36" t="s">
+        <v>360</v>
+      </c>
+      <c r="N12" s="47" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="40" t="s">
         <v>339</v>
       </c>
-      <c r="B13" s="53" t="s">
-        <v>385</v>
-      </c>
-      <c r="C13" s="52" t="s">
-        <v>371</v>
+      <c r="B13" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>370</v>
       </c>
       <c r="D13" t="s">
         <v>338</v>
       </c>
-      <c r="H13" s="48"/>
+      <c r="H13" s="45"/>
       <c r="K13" s="31"/>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
-        <v>348</v>
+      <c r="A14" s="40" t="s">
+        <v>347</v>
       </c>
       <c r="B14" s="31" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
+        <v>362</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>363</v>
+      </c>
+      <c r="D15" s="31" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
-        <v>363</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>347</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>364</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>366</v>
-      </c>
-    </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E16" s="47"/>
-    </row>
-    <row r="22" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="44"/>
+    </row>
+    <row r="17" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="44"/>
+    </row>
+    <row r="22" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="14"/>
     </row>
-    <row r="23" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="51"/>
+    <row r="23" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="48"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
uat reintegro arreglo de ceros
</commit_message>
<xml_diff>
--- a/CuentasUAT.xlsx
+++ b/CuentasUAT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15768" windowHeight="13152" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15768" windowHeight="13152" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -2234,7 +2234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -4758,8 +4758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5238,7 +5238,7 @@
         <v>414</v>
       </c>
       <c r="B20">
-        <v>22222200</v>
+        <v>22222000</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>365</v>
@@ -5258,7 +5258,7 @@
         <v>414</v>
       </c>
       <c r="B21">
-        <v>22222200</v>
+        <v>22222000</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>365</v>
@@ -5278,7 +5278,7 @@
         <v>421</v>
       </c>
       <c r="B22">
-        <v>22222201</v>
+        <v>22222001</v>
       </c>
       <c r="C22" s="14"/>
     </row>
@@ -5287,7 +5287,7 @@
         <v>419</v>
       </c>
       <c r="B23">
-        <v>22222200</v>
+        <v>22222000</v>
       </c>
       <c r="C23" s="47"/>
     </row>
@@ -5296,7 +5296,7 @@
         <v>420</v>
       </c>
       <c r="B24">
-        <v>22222200</v>
+        <v>22222000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>